<commit_message>
fixing some error scnarios
</commit_message>
<xml_diff>
--- a/prod_manage_QA/mobile_manual_testing/acceptence_testing/TST_ACEITACAO_ProdManage_19-09-2024.xlsx
+++ b/prod_manage_QA/mobile_manual_testing/acceptence_testing/TST_ACEITACAO_ProdManage_19-09-2024.xlsx
@@ -62,7 +62,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1526" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1528" uniqueCount="47">
   <si>
     <t>Projeto</t>
   </si>
@@ -167,9 +167,6 @@
     <t>Maria Luisa</t>
   </si>
   <si>
-    <t>NOK</t>
-  </si>
-  <si>
     <t>"o cronômetro de rendimento é confuso, mas de resto está tudo ok"</t>
   </si>
   <si>
@@ -213,6 +210,9 @@
   </si>
   <si>
     <t>Novo cenário de aceitação.</t>
+  </si>
+  <si>
+    <t>Alterando cenário para OK</t>
   </si>
 </sst>
 </file>
@@ -605,7 +605,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="45">
+  <cellXfs count="48">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
@@ -690,6 +690,15 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="14" fontId="0" fillId="2" borderId="21" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -709,13 +718,13 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="2" borderId="21" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -901,10 +910,10 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>2</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>0</c:v>
@@ -1268,7 +1277,7 @@
   <dimension ref="A1:G7"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="D22" sqref="D22"/>
+      <selection activeCell="G27" sqref="G27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1291,11 +1300,11 @@
       <c r="B2" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="E2" s="36" t="s">
+      <c r="E2" s="39" t="s">
         <v>5</v>
       </c>
-      <c r="F2" s="37"/>
-      <c r="G2" s="38"/>
+      <c r="F2" s="40"/>
+      <c r="G2" s="41"/>
     </row>
     <row r="3" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" s="9" t="s">
@@ -1321,14 +1330,14 @@
       <c r="B4" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="E4" s="42">
+      <c r="E4" s="36">
         <v>45564</v>
       </c>
-      <c r="F4" s="43" t="s">
+      <c r="F4" s="37" t="s">
         <v>30</v>
       </c>
-      <c r="G4" s="44" t="s">
-        <v>46</v>
+      <c r="G4" s="38" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
@@ -1338,9 +1347,15 @@
       <c r="B5" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="E5" s="24"/>
-      <c r="F5" s="6"/>
-      <c r="G5" s="25"/>
+      <c r="E5" s="45">
+        <v>45571</v>
+      </c>
+      <c r="F5" s="46" t="s">
+        <v>30</v>
+      </c>
+      <c r="G5" s="47" t="s">
+        <v>46</v>
+      </c>
     </row>
     <row r="6" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A6" s="9" t="s">
@@ -1379,7 +1394,7 @@
   <dimension ref="A1:G1494"/>
   <sheetViews>
     <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+      <selection activeCell="K4" sqref="K4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1431,10 +1446,10 @@
         <v>27</v>
       </c>
       <c r="E2" s="30" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F2" s="30" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="G2" s="30" t="s">
         <v>32</v>
@@ -1445,22 +1460,22 @@
         <v>2</v>
       </c>
       <c r="B3" s="30" t="s">
+        <v>34</v>
+      </c>
+      <c r="C3" s="30" t="s">
         <v>35</v>
       </c>
-      <c r="C3" s="30" t="s">
+      <c r="D3" s="15" t="s">
+        <v>37</v>
+      </c>
+      <c r="E3" s="35" t="s">
+        <v>43</v>
+      </c>
+      <c r="F3" s="30" t="s">
+        <v>38</v>
+      </c>
+      <c r="G3" s="30" t="s">
         <v>36</v>
-      </c>
-      <c r="D3" s="15" t="s">
-        <v>38</v>
-      </c>
-      <c r="E3" s="35" t="s">
-        <v>44</v>
-      </c>
-      <c r="F3" s="30" t="s">
-        <v>33</v>
-      </c>
-      <c r="G3" s="30" t="s">
-        <v>37</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="150" x14ac:dyDescent="0.25">
@@ -1469,22 +1484,22 @@
         <v>3</v>
       </c>
       <c r="B4" s="33" t="s">
+        <v>40</v>
+      </c>
+      <c r="C4" s="33" t="s">
         <v>41</v>
       </c>
-      <c r="C4" s="33" t="s">
+      <c r="D4" s="15" t="s">
         <v>42</v>
       </c>
-      <c r="D4" s="15" t="s">
-        <v>43</v>
-      </c>
       <c r="E4" s="30" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="F4" s="30" t="s">
+        <v>38</v>
+      </c>
+      <c r="G4" s="30" t="s">
         <v>39</v>
-      </c>
-      <c r="G4" s="30" t="s">
-        <v>40</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
@@ -22409,11 +22424,11 @@
   <sheetData>
     <row r="1" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="1:3" ht="27" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="39" t="s">
+      <c r="A2" s="42" t="s">
         <v>11</v>
       </c>
-      <c r="B2" s="40"/>
-      <c r="C2" s="41"/>
+      <c r="B2" s="43"/>
+      <c r="C2" s="44"/>
     </row>
     <row r="3" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" s="12" t="s">
@@ -22433,11 +22448,11 @@
       </c>
       <c r="B4" s="17">
         <f>COUNTIF(Cenários!F:F,"OK")</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C4" s="20">
         <f>B4/B3</f>
-        <v>0.66666666666666663</v>
+        <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
@@ -22446,11 +22461,11 @@
       </c>
       <c r="B5" s="17">
         <f>COUNTIF(Cenários!F:F,"NOK")</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C5" s="20">
         <f>B5/B3</f>
-        <v>0.33333333333333331</v>
+        <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">

</xml_diff>